<commit_message>
[update] => master data and use effect menu to context main page
</commit_message>
<xml_diff>
--- a/public/excel/PurchaseList.xlsx
+++ b/public/excel/PurchaseList.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+  <si>
+    <t>seq</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -354,10 +357,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+      <c r="A2" s="2">
+        <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -365,28 +371,31 @@
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2">
         <v>100.0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>45.0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>7.0</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>30.0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>18.0</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
+      <c r="A3" s="2">
+        <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -394,28 +403,31 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
         <v>100.0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>45.0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>7.0</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>30.0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>18.0</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>12</v>
+      <c r="J3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
+      <c r="A4" s="2">
+        <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -423,28 +435,31 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
         <v>100.0</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>45.0</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>7.0</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>30.0</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>18.0</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>12</v>
+      <c r="J4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
+      <c r="A5" s="2">
+        <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -452,28 +467,31 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2">
         <v>100.0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>45.0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>7.0</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>30.0</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>18.0</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>12</v>
+      <c r="J5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
+      <c r="A6" s="2">
+        <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -481,139 +499,154 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2">
         <v>100.0</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>45.0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>7.0</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>30.0</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>18.0</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>12</v>
+      <c r="J6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
+      <c r="A7" s="2">
+        <v>6.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2">
         <v>80.0</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>35.0</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>5.6</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>24.0</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>15.4</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>12</v>
+      <c r="J7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
+      <c r="A8" s="2">
+        <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2">
         <v>80.0</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>35.0</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>5.6</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>24.0</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>15.4</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>12</v>
+      <c r="J8" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
+      <c r="A9" s="2">
+        <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
         <v>80.0</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>35.0</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>5.6</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>24.0</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>15.4</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>12</v>
+      <c r="J9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="A10" s="2">
+        <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2">
         <v>80.0</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>35.0</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>5.6</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>24.0</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>15.4</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>12</v>
+      <c r="J10" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>